<commit_message>
Changed back for real
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heric\Desktop\School\Year 4\Semester 1\COSC 304\Ratlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14DC3A3D-AD14-4326-804D-93AAD0392733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70554526-0583-4781-A376-195050B85A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9786DE29-1A79-48C9-97F6-C56E8DACF8C8}"/>
   </bookViews>
@@ -471,6 +471,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -478,24 +496,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -814,7 +814,7 @@
   <dimension ref="A1:H82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:E6"/>
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -868,7 +868,7 @@
       </c>
       <c r="H3">
         <f>SUM(D3:D76)</f>
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -909,11 +909,11 @@
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="22" t="s">
@@ -938,11 +938,11 @@
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="22" t="s">
@@ -1083,11 +1083,11 @@
       <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="22" t="s">
@@ -1187,11 +1187,11 @@
       <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="25"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
     </row>
     <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="22" t="s">
@@ -1274,11 +1274,11 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="19"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="21"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="27"/>
     </row>
     <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="22" t="s">
@@ -1320,11 +1320,11 @@
       <c r="E38" s="11"/>
     </row>
     <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="25"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="27"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="21"/>
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="8"/>
@@ -1348,9 +1348,7 @@
       <c r="C43" s="6">
         <v>2</v>
       </c>
-      <c r="D43" s="10">
-        <v>2</v>
-      </c>
+      <c r="D43" s="10"/>
       <c r="E43" s="11"/>
     </row>
     <row r="44" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1421,11 +1419,11 @@
       <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="19"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="21"/>
+      <c r="A49" s="25"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="27"/>
     </row>
     <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="22" t="s">
@@ -1476,11 +1474,11 @@
       <c r="E53" s="11"/>
     </row>
     <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="25"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="27"/>
+      <c r="A54" s="19"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="21"/>
     </row>
     <row r="55" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="22" t="s">
@@ -1518,11 +1516,11 @@
       <c r="E57" s="7"/>
     </row>
     <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="19"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="21"/>
+      <c r="A58" s="25"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="27"/>
     </row>
     <row r="59" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="12" t="s">
@@ -1786,12 +1784,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="A28:E28"/>
@@ -1804,6 +1796,12 @@
     <mergeCell ref="A50:E50"/>
     <mergeCell ref="A54:E54"/>
     <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Finished browsing products by category
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heric\Desktop\School\Year 4\Semester 1\COSC 304\Ratlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70554526-0583-4781-A376-195050B85A2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2348B75-B88C-41E9-95A0-57D6B16A3A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9786DE29-1A79-48C9-97F6-C56E8DACF8C8}"/>
   </bookViews>
@@ -471,6 +471,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -478,24 +496,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674C5126-D32A-4159-BC57-1A5C39BFEA7B}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -868,7 +868,7 @@
       </c>
       <c r="H3">
         <f>SUM(D3:D76)</f>
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -909,11 +909,11 @@
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="27"/>
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="21"/>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="22" t="s">
@@ -938,11 +938,11 @@
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
+      <c r="A9" s="19"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="21"/>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="22" t="s">
@@ -978,7 +978,9 @@
       <c r="C12" s="6">
         <v>1</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="10">
+        <v>1</v>
+      </c>
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1083,11 +1085,11 @@
       <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="19"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21"/>
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="27"/>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="22" t="s">
@@ -1187,11 +1189,11 @@
       <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="19"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="21"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="27"/>
     </row>
     <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="22" t="s">
@@ -1274,11 +1276,11 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="25"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="27"/>
+      <c r="A35" s="19"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="21"/>
     </row>
     <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="22" t="s">
@@ -1320,11 +1322,11 @@
       <c r="E38" s="11"/>
     </row>
     <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="19"/>
-      <c r="B39" s="20"/>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="21"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="26"/>
+      <c r="C39" s="26"/>
+      <c r="D39" s="26"/>
+      <c r="E39" s="27"/>
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="8"/>
@@ -1419,11 +1421,11 @@
       <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="25"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="27"/>
+      <c r="A49" s="19"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="21"/>
     </row>
     <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="22" t="s">
@@ -1474,11 +1476,11 @@
       <c r="E53" s="11"/>
     </row>
     <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="19"/>
-      <c r="B54" s="20"/>
-      <c r="C54" s="20"/>
-      <c r="D54" s="20"/>
-      <c r="E54" s="21"/>
+      <c r="A54" s="25"/>
+      <c r="B54" s="26"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="26"/>
+      <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="22" t="s">
@@ -1516,11 +1518,11 @@
       <c r="E57" s="7"/>
     </row>
     <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="25"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="27"/>
+      <c r="A58" s="19"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="20"/>
+      <c r="D58" s="20"/>
+      <c r="E58" s="21"/>
     </row>
     <row r="59" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="12" t="s">
@@ -1784,6 +1786,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="A28:E28"/>
@@ -1796,12 +1804,6 @@
     <mergeCell ref="A50:E50"/>
     <mergeCell ref="A54:E54"/>
     <mergeCell ref="A55:E55"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated checklist after completing reviews
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heric\Desktop\School\Year 4\Semester 1\COSC 304\Ratlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2348B75-B88C-41E9-95A0-57D6B16A3A04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80752275-05BD-4129-B04D-9F34F51CF031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9786DE29-1A79-48C9-97F6-C56E8DACF8C8}"/>
   </bookViews>
@@ -471,6 +471,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -478,24 +496,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674C5126-D32A-4159-BC57-1A5C39BFEA7B}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -868,7 +868,7 @@
       </c>
       <c r="H3">
         <f>SUM(D3:D76)</f>
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -909,11 +909,11 @@
       <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="27"/>
     </row>
     <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="22" t="s">
@@ -938,11 +938,11 @@
       <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="27"/>
     </row>
     <row r="10" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="22" t="s">
@@ -1085,11 +1085,11 @@
       <c r="E19" s="11"/>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="27"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="21"/>
     </row>
     <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="22" t="s">
@@ -1189,11 +1189,11 @@
       <c r="E27" s="11"/>
     </row>
     <row r="28" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="25"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
+      <c r="A28" s="19"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="21"/>
     </row>
     <row r="29" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="22" t="s">
@@ -1276,11 +1276,11 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="19"/>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="21"/>
+      <c r="A35" s="25"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="26"/>
+      <c r="D35" s="26"/>
+      <c r="E35" s="27"/>
     </row>
     <row r="36" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="22" t="s">
@@ -1322,11 +1322,11 @@
       <c r="E38" s="11"/>
     </row>
     <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="25"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="27"/>
+      <c r="A39" s="19"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="21"/>
     </row>
     <row r="41" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="8"/>
@@ -1421,11 +1421,11 @@
       <c r="E48" s="7"/>
     </row>
     <row r="49" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A49" s="19"/>
-      <c r="B49" s="20"/>
-      <c r="C49" s="20"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="21"/>
+      <c r="A49" s="25"/>
+      <c r="B49" s="26"/>
+      <c r="C49" s="26"/>
+      <c r="D49" s="26"/>
+      <c r="E49" s="27"/>
     </row>
     <row r="50" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="22" t="s">
@@ -1446,7 +1446,9 @@
       <c r="C51" s="6">
         <v>2</v>
       </c>
-      <c r="D51" s="10"/>
+      <c r="D51" s="10">
+        <v>2</v>
+      </c>
       <c r="E51" s="11"/>
     </row>
     <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1459,7 +1461,9 @@
       <c r="C52" s="6">
         <v>1</v>
       </c>
-      <c r="D52" s="10"/>
+      <c r="D52" s="10">
+        <v>1</v>
+      </c>
       <c r="E52" s="11"/>
     </row>
     <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1472,15 +1476,17 @@
       <c r="C53" s="6">
         <v>2</v>
       </c>
-      <c r="D53" s="10"/>
+      <c r="D53" s="10">
+        <v>2</v>
+      </c>
       <c r="E53" s="11"/>
     </row>
     <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A54" s="25"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="26"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="27"/>
+      <c r="A54" s="19"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="21"/>
     </row>
     <row r="55" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="22" t="s">
@@ -1518,11 +1524,11 @@
       <c r="E57" s="7"/>
     </row>
     <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="19"/>
-      <c r="B58" s="20"/>
-      <c r="C58" s="20"/>
-      <c r="D58" s="20"/>
-      <c r="E58" s="21"/>
+      <c r="A58" s="25"/>
+      <c r="B58" s="26"/>
+      <c r="C58" s="26"/>
+      <c r="D58" s="26"/>
+      <c r="E58" s="27"/>
     </row>
     <row r="59" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="12" t="s">
@@ -1786,12 +1792,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A9:E9"/>
-    <mergeCell ref="A10:E10"/>
     <mergeCell ref="A58:E58"/>
     <mergeCell ref="A21:E21"/>
     <mergeCell ref="A28:E28"/>
@@ -1804,6 +1804,12 @@
     <mergeCell ref="A50:E50"/>
     <mergeCell ref="A54:E54"/>
     <mergeCell ref="A55:E55"/>
+    <mergeCell ref="A20:E20"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated checklist for chase
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heric\Desktop\School\Year 4\Semester 1\COSC 304\Ratlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0CFC2B-4428-4E8D-8157-74AFAD0CD792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0FCD03-D47C-4410-9CC9-68B687861C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9786DE29-1A79-48C9-97F6-C56E8DACF8C8}"/>
   </bookViews>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674C5126-D32A-4159-BC57-1A5C39BFEA7B}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -868,7 +868,7 @@
       </c>
       <c r="H3">
         <f>SUM(D3:D76)</f>
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1511,7 +1511,9 @@
       <c r="C56" s="6">
         <v>2</v>
       </c>
-      <c r="D56" s="9"/>
+      <c r="D56" s="9">
+        <v>2</v>
+      </c>
       <c r="E56" s="7"/>
     </row>
     <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Finished updating and removing products for admins
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heric\Desktop\School\Year 4\Semester 1\COSC 304\Ratlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0FCD03-D47C-4410-9CC9-68B687861C08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D174CBF9-1302-4E5E-81EF-E608EAC82B24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9786DE29-1A79-48C9-97F6-C56E8DACF8C8}"/>
   </bookViews>
@@ -813,8 +813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674C5126-D32A-4159-BC57-1A5C39BFEA7B}">
   <dimension ref="A1:H82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -868,7 +868,7 @@
       </c>
       <c r="H3">
         <f>SUM(D3:D76)</f>
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1628,7 +1628,9 @@
       <c r="C65" s="6">
         <v>2</v>
       </c>
-      <c r="D65" s="10"/>
+      <c r="D65" s="10">
+        <v>2</v>
+      </c>
       <c r="E65" s="11"/>
     </row>
     <row r="66" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
Admin page now requires admin auth
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heric\Desktop\School\Year 4\Semester 1\COSC 304\Ratlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8216463D-A20E-40AA-806E-F2FD1E4B3476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED11163-9A06-4864-B40A-BE396958D381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9786DE29-1A79-48C9-97F6-C56E8DACF8C8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
   <si>
     <t>Final Overall System Features</t>
   </si>
@@ -267,6 +267,42 @@
   </si>
   <si>
     <t>List of Web and AI sources used</t>
+  </si>
+  <si>
+    <t>listprod.jsp</t>
+  </si>
+  <si>
+    <t>product.jsp</t>
+  </si>
+  <si>
+    <t>HTML on all pages</t>
+  </si>
+  <si>
+    <t>Very pretty</t>
+  </si>
+  <si>
+    <t>showcart.jsp</t>
+  </si>
+  <si>
+    <t>checkout.jsp</t>
+  </si>
+  <si>
+    <t>register.html</t>
+  </si>
+  <si>
+    <t>processRegistration.jsp</t>
+  </si>
+  <si>
+    <t>customer.jsp</t>
+  </si>
+  <si>
+    <t>login.jsp/logout.jsp</t>
+  </si>
+  <si>
+    <t>product.jsp/processReview.jsp</t>
+  </si>
+  <si>
+    <t>processReview.jsp</t>
   </si>
 </sst>
 </file>
@@ -816,13 +852,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674C5126-D32A-4159-BC57-1A5C39BFEA7B}">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="40.6328125" customWidth="1"/>
+    <col min="5" max="5" width="28.453125" customWidth="1"/>
     <col min="7" max="7" width="30" customWidth="1"/>
   </cols>
   <sheetData>
@@ -984,7 +1021,9 @@
       <c r="D12" s="10">
         <v>1</v>
       </c>
-      <c r="E12" s="11"/>
+      <c r="E12" s="11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="5" t="s">
@@ -999,7 +1038,9 @@
       <c r="D13" s="10">
         <v>1</v>
       </c>
-      <c r="E13" s="11"/>
+      <c r="E13" s="11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5" t="s">
@@ -1014,7 +1055,9 @@
       <c r="D14" s="10">
         <v>1</v>
       </c>
-      <c r="E14" s="11"/>
+      <c r="E14" s="11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="5" t="s">
@@ -1029,7 +1072,9 @@
       <c r="D15" s="10">
         <v>1</v>
       </c>
-      <c r="E15" s="11"/>
+      <c r="E15" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="5" t="s">
@@ -1044,7 +1089,9 @@
       <c r="D16" s="10">
         <v>1</v>
       </c>
-      <c r="E16" s="11"/>
+      <c r="E16" s="11" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="5" t="s">
@@ -1087,7 +1134,9 @@
       <c r="D19" s="10">
         <v>2</v>
       </c>
-      <c r="E19" s="11"/>
+      <c r="E19" s="11" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="5" t="s">
@@ -1131,7 +1180,9 @@
       <c r="D23" s="10">
         <v>1</v>
       </c>
-      <c r="E23" s="11"/>
+      <c r="E23" s="11" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="5" t="s">
@@ -1146,7 +1197,9 @@
       <c r="D24" s="10">
         <v>1</v>
       </c>
-      <c r="E24" s="11"/>
+      <c r="E24" s="11" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
@@ -1161,7 +1214,9 @@
       <c r="D25" s="10">
         <v>1</v>
       </c>
-      <c r="E25" s="11"/>
+      <c r="E25" s="11" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="5" t="s">
@@ -1176,7 +1231,9 @@
       <c r="D26" s="10">
         <v>1</v>
       </c>
-      <c r="E26" s="11"/>
+      <c r="E26" s="11" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="27" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="5" t="s">
@@ -1235,7 +1292,9 @@
       <c r="D31" s="10">
         <v>1</v>
       </c>
-      <c r="E31" s="11"/>
+      <c r="E31" s="11" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="5" t="s">
@@ -1322,7 +1381,9 @@
       <c r="D38" s="10">
         <v>1</v>
       </c>
-      <c r="E38" s="11"/>
+      <c r="E38" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="5" t="s">
@@ -1337,7 +1398,9 @@
       <c r="D39" s="10">
         <v>1</v>
       </c>
-      <c r="E39" s="11"/>
+      <c r="E39" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="40" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="25"/>
@@ -1371,9 +1434,11 @@
       <c r="D44" s="10">
         <v>2</v>
       </c>
-      <c r="E44" s="11"/>
-    </row>
-    <row r="45" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E44" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="5" t="s">
         <v>43</v>
       </c>
@@ -1386,7 +1451,9 @@
       <c r="D45" s="10">
         <v>2</v>
       </c>
-      <c r="E45" s="11"/>
+      <c r="E45" s="11" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="46" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="5" t="s">
@@ -1401,7 +1468,9 @@
       <c r="D46" s="10">
         <v>2</v>
       </c>
-      <c r="E46" s="11"/>
+      <c r="E46" s="11" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="5" t="s">
@@ -1416,7 +1485,9 @@
       <c r="D47" s="10">
         <v>1</v>
       </c>
-      <c r="E47" s="11"/>
+      <c r="E47" s="11" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="48" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="5" t="s">
@@ -1460,7 +1531,7 @@
       <c r="D51" s="23"/>
       <c r="E51" s="24"/>
     </row>
-    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="5" t="s">
         <v>49</v>
       </c>
@@ -1473,7 +1544,9 @@
       <c r="D52" s="10">
         <v>2</v>
       </c>
-      <c r="E52" s="11"/>
+      <c r="E52" s="11" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="53" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="5" t="s">
@@ -1488,7 +1561,9 @@
       <c r="D53" s="10">
         <v>1</v>
       </c>
-      <c r="E53" s="11"/>
+      <c r="E53" s="11" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="5" t="s">
@@ -1503,7 +1578,9 @@
       <c r="D54" s="10">
         <v>2</v>
       </c>
-      <c r="E54" s="11"/>
+      <c r="E54" s="11" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="55" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="25"/>
@@ -1534,7 +1611,9 @@
       <c r="D57" s="9">
         <v>2</v>
       </c>
-      <c r="E57" s="7"/>
+      <c r="E57" s="7" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="5" t="s">

</xml_diff>

<commit_message>
Added customer list to admin
</commit_message>
<xml_diff>
--- a/CheckList.xlsx
+++ b/CheckList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\heric\Desktop\School\Year 4\Semester 1\COSC 304\Ratlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A40AC436-5FBA-4690-B090-3D4306DF77D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B342187B-42E3-45B2-966F-45A1F65127AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{9786DE29-1A79-48C9-97F6-C56E8DACF8C8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="93">
   <si>
     <t>Final Overall System Features</t>
   </si>
@@ -864,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{674C5126-D32A-4159-BC57-1A5C39BFEA7B}">
   <dimension ref="A1:H83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -920,7 +920,7 @@
       </c>
       <c r="H3">
         <f>SUM(D3:D77)</f>
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1625,7 +1625,7 @@
       <c r="D57" s="9">
         <v>2</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="E57" s="11" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1685,8 +1685,12 @@
       <c r="C62" s="6">
         <v>1</v>
       </c>
-      <c r="D62" s="10"/>
-      <c r="E62" s="11"/>
+      <c r="D62" s="10">
+        <v>1</v>
+      </c>
+      <c r="E62" s="11" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="5" t="s">

</xml_diff>